<commit_message>
DSA Leaning Calendar Plan
</commit_message>
<xml_diff>
--- a/Learning Calendar.xlsx
+++ b/Learning Calendar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code-and-learn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{023A6BCB-49B7-4FF2-8163-F5C366DE9CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5BEE53-51D3-44CC-9D7C-149799ED2712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{84E1BF53-7EDF-4571-BF96-89F7C2236339}"/>
   </bookViews>
@@ -108,10 +108,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,7 +429,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -440,15 +440,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -489,7 +489,7 @@
       <c r="E3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>45502</v>
       </c>
       <c r="G3">

</xml_diff>